<commit_message>
Generic Utility Implementation contd...
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sncsr\eclipse-workspace\VtigerCRM_QKP\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B7124B-4211-44D9-B30D-B326F4A34463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C4F670-98F0-44EC-92C8-77D0A73636CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrganizationsTestData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Create Contact With Organization</t>
   </si>
   <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
     <t>Create lead</t>
   </si>
   <si>
@@ -151,12 +148,19 @@
   </si>
   <si>
     <t>Due Date</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -747,18 +751,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.21875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="39.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="29.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -883,17 +887,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -926,7 +930,7 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>19</v>
       </c>
     </row>
@@ -971,9 +975,9 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>19</v>
       </c>
     </row>
@@ -984,7 +988,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1020,11 +1024,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,13 +1053,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -1066,7 +1070,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1105,15 +1109,15 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>19</v>
       </c>
     </row>
@@ -1124,7 +1128,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -1137,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1148,7 +1152,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1180,11 +1184,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1209,15 +1213,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>19</v>
       </c>
     </row>
@@ -1225,10 +1229,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1238,10 +1242,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1249,10 +1253,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Batch and Group executions done
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -840,7 +840,7 @@
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s" s="1">
         <v>19</v>
       </c>
     </row>

</xml_diff>